<commit_message>
Double to Byte transmission - serial.write V1
</commit_message>
<xml_diff>
--- a/MAIN/2021_11_21 - 3czujniki ludzik leonardo/SD_timetest_changing_euler_probe/SD_time_test_probe/SD_115200_200_vector_euler_NewLibrary.xlsx
+++ b/MAIN/2021_11_21 - 3czujniki ludzik leonardo/SD_timetest_changing_euler_probe/SD_time_test_probe/SD_115200_200_vector_euler_NewLibrary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Motion\Motion-capture\MAIN\2021_11_21 - 3czujniki ludzik leonardo\SD_timetest_changing_euler_probe\SD_time_test_probe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB88B61C-68C8-4315-B16E-CC80D1DBA903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9925EF91-3695-4902-A4F7-34AD2E8E83DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B08684A0-21EF-45A2-A62C-E10381DA47C4}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B08684A0-21EF-45A2-A62C-E10381DA47C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>delta12[μs]</t>
   </si>
@@ -436,13 +436,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59795E7-8513-4965-8627-7A6C21FB21B5}">
-  <dimension ref="A1:AB203"/>
+  <dimension ref="A1:AB204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E190" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P206" sqref="P205:Q206"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z204" sqref="Z204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="22" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="V1" t="s">
@@ -19109,6 +19115,15 @@
         <v>8</v>
       </c>
     </row>
+    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z204">
+        <f>1/Z203</f>
+        <v>63.652994427816864</v>
+      </c>
+      <c r="AA204" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New idea of code, every sensors will have own object bno, final speed transmission measurment
</commit_message>
<xml_diff>
--- a/MAIN/2021_11_21 - 3czujniki ludzik leonardo/SD_timetest_changing_euler_probe/SD_time_test_probe/SD_115200_200_vector_euler_NewLibrary.xlsx
+++ b/MAIN/2021_11_21 - 3czujniki ludzik leonardo/SD_timetest_changing_euler_probe/SD_time_test_probe/SD_115200_200_vector_euler_NewLibrary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Motion\Motion-capture\MAIN\2021_11_21 - 3czujniki ludzik leonardo\SD_timetest_changing_euler_probe\SD_time_test_probe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9925EF91-3695-4902-A4F7-34AD2E8E83DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801828C7-D05E-4296-B46E-9D65F5B024F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B08684A0-21EF-45A2-A62C-E10381DA47C4}"/>
   </bookViews>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59795E7-8513-4965-8627-7A6C21FB21B5}">
   <dimension ref="A1:AB204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z204" sqref="Z204"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V202" sqref="V1:AB202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>